<commit_message>
Modify XML + xlsx file
- Modify PrisonBreak.xml
- Modify xlsx of this
</commit_message>
<xml_diff>
--- a/MovieSimulator/MovieSimulator/XML/PrisonBreak.xlsx
+++ b/MovieSimulator/MovieSimulator/XML/PrisonBreak.xlsx
@@ -23,13 +23,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,15 +33,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -55,18 +44,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -84,25 +61,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3300"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF663300"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,17 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +388,7 @@
   <dimension ref="CV100:DO119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CV100" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="DH103" sqref="DH103:DL106"/>
+      <selection activeCell="DC108" sqref="DC108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -463,38 +417,38 @@
     </row>
     <row r="101" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CV101" s="1"/>
-      <c r="CW101" s="2"/>
-      <c r="CX101" s="2"/>
-      <c r="CY101" s="2"/>
-      <c r="CZ101" s="2"/>
-      <c r="DA101" s="2"/>
-      <c r="DB101" s="2"/>
-      <c r="DC101" s="2"/>
-      <c r="DD101" s="2"/>
-      <c r="DE101" s="3"/>
-      <c r="DF101" s="5"/>
-      <c r="DG101" s="5"/>
-      <c r="DH101" s="5"/>
-      <c r="DI101" s="5"/>
-      <c r="DJ101" s="5"/>
-      <c r="DK101" s="5"/>
-      <c r="DL101" s="5"/>
-      <c r="DM101" s="5"/>
-      <c r="DN101" s="5"/>
+      <c r="CW101" s="3"/>
+      <c r="CX101" s="3"/>
+      <c r="CY101" s="3"/>
+      <c r="CZ101" s="3"/>
+      <c r="DA101" s="3"/>
+      <c r="DB101" s="3"/>
+      <c r="DC101" s="3"/>
+      <c r="DD101" s="3"/>
+      <c r="DE101" s="2"/>
+      <c r="DF101" s="3"/>
+      <c r="DG101" s="3"/>
+      <c r="DH101" s="3"/>
+      <c r="DI101" s="3"/>
+      <c r="DJ101" s="3"/>
+      <c r="DK101" s="3"/>
+      <c r="DL101" s="3"/>
+      <c r="DM101" s="3"/>
+      <c r="DN101" s="3"/>
       <c r="DO101" s="1"/>
     </row>
     <row r="102" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CV102" s="1"/>
-      <c r="CW102" s="2"/>
-      <c r="CX102" s="2"/>
-      <c r="CY102" s="2"/>
-      <c r="CZ102" s="2"/>
-      <c r="DA102" s="2"/>
-      <c r="DB102" s="2"/>
-      <c r="DC102" s="2"/>
-      <c r="DD102" s="2"/>
-      <c r="DE102" s="3"/>
-      <c r="DF102" s="5"/>
+      <c r="CW102" s="3"/>
+      <c r="CX102" s="3"/>
+      <c r="CY102" s="3"/>
+      <c r="CZ102" s="3"/>
+      <c r="DA102" s="3"/>
+      <c r="DB102" s="3"/>
+      <c r="DC102" s="3"/>
+      <c r="DD102" s="3"/>
+      <c r="DE102" s="2"/>
+      <c r="DF102" s="3"/>
       <c r="DG102" s="1"/>
       <c r="DH102" s="1"/>
       <c r="DI102" s="1"/>
@@ -502,51 +456,51 @@
       <c r="DK102" s="1"/>
       <c r="DL102" s="1"/>
       <c r="DM102" s="1"/>
-      <c r="DN102" s="5"/>
+      <c r="DN102" s="3"/>
       <c r="DO102" s="1"/>
     </row>
     <row r="103" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CV103" s="1"/>
-      <c r="CW103" s="3"/>
-      <c r="CX103" s="3"/>
-      <c r="CY103" s="3"/>
-      <c r="CZ103" s="3"/>
-      <c r="DA103" s="3"/>
-      <c r="DB103" s="3"/>
-      <c r="DC103" s="3"/>
-      <c r="DD103" s="8"/>
-      <c r="DE103" s="3"/>
-      <c r="DF103" s="5"/>
+      <c r="CW103" s="2"/>
+      <c r="CX103" s="2"/>
+      <c r="CY103" s="2"/>
+      <c r="CZ103" s="2"/>
+      <c r="DA103" s="2"/>
+      <c r="DB103" s="2"/>
+      <c r="DC103" s="2"/>
+      <c r="DD103" s="4"/>
+      <c r="DE103" s="2"/>
+      <c r="DF103" s="3"/>
       <c r="DG103" s="1"/>
-      <c r="DH103" s="9"/>
-      <c r="DI103" s="9"/>
-      <c r="DJ103" s="9"/>
-      <c r="DK103" s="9"/>
-      <c r="DL103" s="9"/>
-      <c r="DM103" s="8"/>
-      <c r="DN103" s="5"/>
+      <c r="DH103" s="3"/>
+      <c r="DI103" s="3"/>
+      <c r="DJ103" s="3"/>
+      <c r="DK103" s="3"/>
+      <c r="DL103" s="3"/>
+      <c r="DM103" s="4"/>
+      <c r="DN103" s="3"/>
       <c r="DO103" s="1"/>
     </row>
     <row r="104" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CV104" s="1"/>
-      <c r="CW104" s="5"/>
-      <c r="CX104" s="5"/>
-      <c r="CY104" s="5"/>
-      <c r="CZ104" s="5"/>
-      <c r="DA104" s="5"/>
-      <c r="DB104" s="5"/>
-      <c r="DC104" s="5"/>
-      <c r="DD104" s="5"/>
-      <c r="DE104" s="5"/>
-      <c r="DF104" s="5"/>
+      <c r="CW104" s="3"/>
+      <c r="CX104" s="3"/>
+      <c r="CY104" s="3"/>
+      <c r="CZ104" s="3"/>
+      <c r="DA104" s="3"/>
+      <c r="DB104" s="3"/>
+      <c r="DC104" s="3"/>
+      <c r="DD104" s="3"/>
+      <c r="DE104" s="3"/>
+      <c r="DF104" s="3"/>
       <c r="DG104" s="1"/>
-      <c r="DH104" s="9"/>
-      <c r="DI104" s="9"/>
-      <c r="DJ104" s="9"/>
-      <c r="DK104" s="9"/>
-      <c r="DL104" s="9"/>
+      <c r="DH104" s="3"/>
+      <c r="DI104" s="3"/>
+      <c r="DJ104" s="3"/>
+      <c r="DK104" s="3"/>
+      <c r="DL104" s="3"/>
       <c r="DM104" s="1"/>
-      <c r="DN104" s="5"/>
+      <c r="DN104" s="3"/>
       <c r="DO104" s="1"/>
     </row>
     <row r="105" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -562,51 +516,51 @@
       <c r="DE105" s="1"/>
       <c r="DF105" s="1"/>
       <c r="DG105" s="1"/>
-      <c r="DH105" s="9"/>
-      <c r="DI105" s="9"/>
-      <c r="DJ105" s="9"/>
-      <c r="DK105" s="9"/>
-      <c r="DL105" s="9"/>
+      <c r="DH105" s="3"/>
+      <c r="DI105" s="3"/>
+      <c r="DJ105" s="3"/>
+      <c r="DK105" s="3"/>
+      <c r="DL105" s="3"/>
       <c r="DM105" s="1"/>
-      <c r="DN105" s="5"/>
+      <c r="DN105" s="3"/>
       <c r="DO105" s="1"/>
     </row>
     <row r="106" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV106" s="7"/>
-      <c r="CW106" s="7"/>
-      <c r="CX106" s="7"/>
-      <c r="CY106" s="7"/>
-      <c r="CZ106" s="7"/>
-      <c r="DA106" s="7"/>
+      <c r="CV106" s="3"/>
+      <c r="CW106" s="3"/>
+      <c r="CX106" s="3"/>
+      <c r="CY106" s="3"/>
+      <c r="CZ106" s="3"/>
+      <c r="DA106" s="3"/>
       <c r="DB106" s="1"/>
-      <c r="DC106" s="4"/>
-      <c r="DD106" s="4"/>
-      <c r="DE106" s="4"/>
-      <c r="DF106" s="4"/>
+      <c r="DC106" s="3"/>
+      <c r="DD106" s="3"/>
+      <c r="DE106" s="3"/>
+      <c r="DF106" s="3"/>
       <c r="DG106" s="1"/>
-      <c r="DH106" s="9"/>
-      <c r="DI106" s="9"/>
-      <c r="DJ106" s="9"/>
-      <c r="DK106" s="9"/>
-      <c r="DL106" s="9"/>
+      <c r="DH106" s="3"/>
+      <c r="DI106" s="3"/>
+      <c r="DJ106" s="3"/>
+      <c r="DK106" s="3"/>
+      <c r="DL106" s="3"/>
       <c r="DM106" s="1"/>
-      <c r="DN106" s="5"/>
+      <c r="DN106" s="3"/>
       <c r="DO106" s="1"/>
     </row>
     <row r="107" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV107" s="7"/>
-      <c r="CW107" s="7"/>
-      <c r="CX107" s="7"/>
-      <c r="CY107" s="7"/>
-      <c r="CZ107" s="7"/>
-      <c r="DA107" s="7"/>
+      <c r="CV107" s="3"/>
+      <c r="CW107" s="3"/>
+      <c r="CX107" s="3"/>
+      <c r="CY107" s="3"/>
+      <c r="CZ107" s="3"/>
+      <c r="DA107" s="3"/>
       <c r="DB107" s="1"/>
-      <c r="DC107" s="4"/>
-      <c r="DD107" s="4"/>
-      <c r="DE107" s="4"/>
-      <c r="DF107" s="4"/>
+      <c r="DC107" s="3"/>
+      <c r="DD107" s="3"/>
+      <c r="DE107" s="3"/>
+      <c r="DF107" s="3"/>
       <c r="DG107" s="1"/>
-      <c r="DH107" s="8"/>
+      <c r="DH107" s="4"/>
       <c r="DI107" s="1"/>
       <c r="DJ107" s="1"/>
       <c r="DK107" s="1"/>
@@ -616,254 +570,254 @@
       <c r="DO107" s="1"/>
     </row>
     <row r="108" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV108" s="7"/>
-      <c r="CW108" s="7"/>
-      <c r="CX108" s="7"/>
-      <c r="CY108" s="7"/>
-      <c r="CZ108" s="7"/>
-      <c r="DA108" s="7"/>
+      <c r="CV108" s="3"/>
+      <c r="CW108" s="3"/>
+      <c r="CX108" s="3"/>
+      <c r="CY108" s="3"/>
+      <c r="CZ108" s="3"/>
+      <c r="DA108" s="3"/>
       <c r="DB108" s="1"/>
-      <c r="DC108" s="4"/>
-      <c r="DD108" s="4"/>
-      <c r="DE108" s="4"/>
-      <c r="DF108" s="4"/>
+      <c r="DC108" s="3"/>
+      <c r="DD108" s="3"/>
+      <c r="DE108" s="3"/>
+      <c r="DF108" s="3"/>
       <c r="DG108" s="1"/>
-      <c r="DH108" s="4"/>
+      <c r="DH108" s="3"/>
       <c r="DI108" s="1"/>
-      <c r="DJ108" s="4"/>
-      <c r="DK108" s="4"/>
-      <c r="DL108" s="4"/>
-      <c r="DM108" s="4"/>
-      <c r="DN108" s="4"/>
+      <c r="DJ108" s="3"/>
+      <c r="DK108" s="3"/>
+      <c r="DL108" s="3"/>
+      <c r="DM108" s="3"/>
+      <c r="DN108" s="3"/>
       <c r="DO108" s="1"/>
     </row>
     <row r="109" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV109" s="7"/>
-      <c r="CW109" s="7"/>
-      <c r="CX109" s="7"/>
-      <c r="CY109" s="7"/>
-      <c r="CZ109" s="7"/>
-      <c r="DA109" s="7"/>
+      <c r="CV109" s="3"/>
+      <c r="CW109" s="3"/>
+      <c r="CX109" s="3"/>
+      <c r="CY109" s="3"/>
+      <c r="CZ109" s="3"/>
+      <c r="DA109" s="3"/>
       <c r="DB109" s="1"/>
-      <c r="DC109" s="4"/>
-      <c r="DD109" s="4"/>
-      <c r="DE109" s="4"/>
-      <c r="DF109" s="4"/>
+      <c r="DC109" s="3"/>
+      <c r="DD109" s="3"/>
+      <c r="DE109" s="3"/>
+      <c r="DF109" s="3"/>
       <c r="DG109" s="1"/>
-      <c r="DH109" s="4"/>
+      <c r="DH109" s="3"/>
       <c r="DI109" s="1"/>
-      <c r="DJ109" s="4"/>
-      <c r="DK109" s="4"/>
-      <c r="DL109" s="4"/>
-      <c r="DM109" s="4"/>
-      <c r="DN109" s="4"/>
+      <c r="DJ109" s="3"/>
+      <c r="DK109" s="3"/>
+      <c r="DL109" s="3"/>
+      <c r="DM109" s="3"/>
+      <c r="DN109" s="3"/>
       <c r="DO109" s="1"/>
     </row>
     <row r="110" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV110" s="7"/>
-      <c r="CW110" s="7"/>
-      <c r="CX110" s="7"/>
-      <c r="CY110" s="7"/>
-      <c r="CZ110" s="7"/>
-      <c r="DA110" s="7"/>
+      <c r="CV110" s="3"/>
+      <c r="CW110" s="3"/>
+      <c r="CX110" s="3"/>
+      <c r="CY110" s="3"/>
+      <c r="CZ110" s="3"/>
+      <c r="DA110" s="3"/>
       <c r="DB110" s="1"/>
-      <c r="DC110" s="4"/>
-      <c r="DD110" s="4"/>
-      <c r="DE110" s="4"/>
-      <c r="DF110" s="4"/>
+      <c r="DC110" s="3"/>
+      <c r="DD110" s="3"/>
+      <c r="DE110" s="3"/>
+      <c r="DF110" s="3"/>
       <c r="DG110" s="1"/>
-      <c r="DH110" s="8"/>
+      <c r="DH110" s="4"/>
       <c r="DI110" s="1"/>
-      <c r="DJ110" s="4"/>
-      <c r="DK110" s="4"/>
-      <c r="DL110" s="4"/>
-      <c r="DM110" s="4"/>
-      <c r="DN110" s="4"/>
+      <c r="DJ110" s="3"/>
+      <c r="DK110" s="3"/>
+      <c r="DL110" s="3"/>
+      <c r="DM110" s="3"/>
+      <c r="DN110" s="3"/>
       <c r="DO110" s="1"/>
     </row>
     <row r="111" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV111" s="6"/>
-      <c r="CW111" s="6"/>
-      <c r="CX111" s="7"/>
-      <c r="CY111" s="7"/>
-      <c r="CZ111" s="7"/>
-      <c r="DA111" s="7"/>
+      <c r="CV111" s="3"/>
+      <c r="CW111" s="3"/>
+      <c r="CX111" s="3"/>
+      <c r="CY111" s="3"/>
+      <c r="CZ111" s="3"/>
+      <c r="DA111" s="3"/>
       <c r="DB111" s="1"/>
-      <c r="DC111" s="4"/>
-      <c r="DD111" s="4"/>
-      <c r="DE111" s="4"/>
-      <c r="DF111" s="4"/>
-      <c r="DG111" s="4"/>
-      <c r="DH111" s="4"/>
-      <c r="DI111" s="4"/>
-      <c r="DJ111" s="4"/>
-      <c r="DK111" s="4"/>
-      <c r="DL111" s="4"/>
-      <c r="DM111" s="4"/>
-      <c r="DN111" s="4"/>
+      <c r="DC111" s="3"/>
+      <c r="DD111" s="3"/>
+      <c r="DE111" s="3"/>
+      <c r="DF111" s="3"/>
+      <c r="DG111" s="3"/>
+      <c r="DH111" s="3"/>
+      <c r="DI111" s="3"/>
+      <c r="DJ111" s="3"/>
+      <c r="DK111" s="3"/>
+      <c r="DL111" s="3"/>
+      <c r="DM111" s="3"/>
+      <c r="DN111" s="3"/>
       <c r="DO111" s="1"/>
     </row>
     <row r="112" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV112" s="6"/>
-      <c r="CW112" s="6"/>
-      <c r="CX112" s="7"/>
-      <c r="CY112" s="7"/>
-      <c r="CZ112" s="7"/>
-      <c r="DA112" s="7"/>
-      <c r="DB112" s="8"/>
-      <c r="DC112" s="4"/>
-      <c r="DD112" s="4"/>
-      <c r="DE112" s="4"/>
-      <c r="DF112" s="4"/>
-      <c r="DG112" s="4"/>
-      <c r="DH112" s="4"/>
-      <c r="DI112" s="4"/>
-      <c r="DJ112" s="4"/>
-      <c r="DK112" s="4"/>
-      <c r="DL112" s="4"/>
-      <c r="DM112" s="4"/>
-      <c r="DN112" s="4"/>
+      <c r="CV112" s="3"/>
+      <c r="CW112" s="3"/>
+      <c r="CX112" s="3"/>
+      <c r="CY112" s="3"/>
+      <c r="CZ112" s="3"/>
+      <c r="DA112" s="3"/>
+      <c r="DB112" s="4"/>
+      <c r="DC112" s="3"/>
+      <c r="DD112" s="3"/>
+      <c r="DE112" s="3"/>
+      <c r="DF112" s="3"/>
+      <c r="DG112" s="3"/>
+      <c r="DH112" s="3"/>
+      <c r="DI112" s="3"/>
+      <c r="DJ112" s="3"/>
+      <c r="DK112" s="3"/>
+      <c r="DL112" s="3"/>
+      <c r="DM112" s="3"/>
+      <c r="DN112" s="3"/>
       <c r="DO112" s="1"/>
     </row>
     <row r="113" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV113" s="6"/>
-      <c r="CW113" s="6"/>
-      <c r="CX113" s="7"/>
-      <c r="CY113" s="7"/>
-      <c r="CZ113" s="7"/>
-      <c r="DA113" s="7"/>
-      <c r="DB113" s="8"/>
-      <c r="DC113" s="4"/>
-      <c r="DD113" s="4"/>
-      <c r="DE113" s="4"/>
-      <c r="DF113" s="4"/>
-      <c r="DG113" s="4"/>
-      <c r="DH113" s="4"/>
-      <c r="DI113" s="4"/>
-      <c r="DJ113" s="4"/>
-      <c r="DK113" s="4"/>
-      <c r="DL113" s="4"/>
-      <c r="DM113" s="4"/>
-      <c r="DN113" s="4"/>
+      <c r="CV113" s="3"/>
+      <c r="CW113" s="3"/>
+      <c r="CX113" s="3"/>
+      <c r="CY113" s="3"/>
+      <c r="CZ113" s="3"/>
+      <c r="DA113" s="3"/>
+      <c r="DB113" s="4"/>
+      <c r="DC113" s="3"/>
+      <c r="DD113" s="3"/>
+      <c r="DE113" s="3"/>
+      <c r="DF113" s="3"/>
+      <c r="DG113" s="3"/>
+      <c r="DH113" s="3"/>
+      <c r="DI113" s="3"/>
+      <c r="DJ113" s="3"/>
+      <c r="DK113" s="3"/>
+      <c r="DL113" s="3"/>
+      <c r="DM113" s="3"/>
+      <c r="DN113" s="3"/>
       <c r="DO113" s="1"/>
     </row>
     <row r="114" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV114" s="6"/>
-      <c r="CW114" s="6"/>
-      <c r="CX114" s="7"/>
-      <c r="CY114" s="7"/>
-      <c r="CZ114" s="7"/>
-      <c r="DA114" s="7"/>
+      <c r="CV114" s="3"/>
+      <c r="CW114" s="3"/>
+      <c r="CX114" s="3"/>
+      <c r="CY114" s="3"/>
+      <c r="CZ114" s="3"/>
+      <c r="DA114" s="3"/>
       <c r="DB114" s="1"/>
-      <c r="DC114" s="4"/>
-      <c r="DD114" s="4"/>
-      <c r="DE114" s="4"/>
-      <c r="DF114" s="4"/>
-      <c r="DG114" s="4"/>
-      <c r="DH114" s="4"/>
-      <c r="DI114" s="4"/>
-      <c r="DJ114" s="4"/>
-      <c r="DK114" s="4"/>
-      <c r="DL114" s="4"/>
-      <c r="DM114" s="4"/>
-      <c r="DN114" s="4"/>
+      <c r="DC114" s="3"/>
+      <c r="DD114" s="3"/>
+      <c r="DE114" s="3"/>
+      <c r="DF114" s="3"/>
+      <c r="DG114" s="3"/>
+      <c r="DH114" s="3"/>
+      <c r="DI114" s="3"/>
+      <c r="DJ114" s="3"/>
+      <c r="DK114" s="3"/>
+      <c r="DL114" s="3"/>
+      <c r="DM114" s="3"/>
+      <c r="DN114" s="3"/>
       <c r="DO114" s="1"/>
     </row>
     <row r="115" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV115" s="7"/>
-      <c r="CW115" s="7"/>
-      <c r="CX115" s="7"/>
-      <c r="CY115" s="7"/>
-      <c r="CZ115" s="7"/>
-      <c r="DA115" s="7"/>
+      <c r="CV115" s="3"/>
+      <c r="CW115" s="3"/>
+      <c r="CX115" s="3"/>
+      <c r="CY115" s="3"/>
+      <c r="CZ115" s="3"/>
+      <c r="DA115" s="3"/>
       <c r="DB115" s="1"/>
-      <c r="DC115" s="4"/>
-      <c r="DD115" s="4"/>
-      <c r="DE115" s="4"/>
-      <c r="DF115" s="4"/>
-      <c r="DG115" s="4"/>
-      <c r="DH115" s="4"/>
-      <c r="DI115" s="4"/>
-      <c r="DJ115" s="4"/>
-      <c r="DK115" s="4"/>
-      <c r="DL115" s="4"/>
-      <c r="DM115" s="4"/>
-      <c r="DN115" s="4"/>
+      <c r="DC115" s="3"/>
+      <c r="DD115" s="3"/>
+      <c r="DE115" s="3"/>
+      <c r="DF115" s="3"/>
+      <c r="DG115" s="3"/>
+      <c r="DH115" s="3"/>
+      <c r="DI115" s="3"/>
+      <c r="DJ115" s="3"/>
+      <c r="DK115" s="3"/>
+      <c r="DL115" s="3"/>
+      <c r="DM115" s="3"/>
+      <c r="DN115" s="3"/>
       <c r="DO115" s="1"/>
     </row>
     <row r="116" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV116" s="7"/>
-      <c r="CW116" s="7"/>
-      <c r="CX116" s="7"/>
-      <c r="CY116" s="7"/>
-      <c r="CZ116" s="7"/>
-      <c r="DA116" s="7"/>
+      <c r="CV116" s="3"/>
+      <c r="CW116" s="3"/>
+      <c r="CX116" s="3"/>
+      <c r="CY116" s="3"/>
+      <c r="CZ116" s="3"/>
+      <c r="DA116" s="3"/>
       <c r="DB116" s="1"/>
-      <c r="DC116" s="4"/>
-      <c r="DD116" s="4"/>
-      <c r="DE116" s="4"/>
-      <c r="DF116" s="4"/>
-      <c r="DG116" s="4"/>
-      <c r="DH116" s="4"/>
-      <c r="DI116" s="4"/>
-      <c r="DJ116" s="4"/>
-      <c r="DK116" s="4"/>
-      <c r="DL116" s="4"/>
-      <c r="DM116" s="4"/>
-      <c r="DN116" s="4"/>
+      <c r="DC116" s="3"/>
+      <c r="DD116" s="3"/>
+      <c r="DE116" s="3"/>
+      <c r="DF116" s="3"/>
+      <c r="DG116" s="3"/>
+      <c r="DH116" s="3"/>
+      <c r="DI116" s="3"/>
+      <c r="DJ116" s="3"/>
+      <c r="DK116" s="3"/>
+      <c r="DL116" s="3"/>
+      <c r="DM116" s="3"/>
+      <c r="DN116" s="3"/>
       <c r="DO116" s="1"/>
     </row>
     <row r="117" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV117" s="7"/>
-      <c r="CW117" s="7"/>
-      <c r="CX117" s="7"/>
-      <c r="CY117" s="7"/>
-      <c r="CZ117" s="7"/>
-      <c r="DA117" s="7"/>
+      <c r="CV117" s="3"/>
+      <c r="CW117" s="3"/>
+      <c r="CX117" s="3"/>
+      <c r="CY117" s="3"/>
+      <c r="CZ117" s="3"/>
+      <c r="DA117" s="3"/>
       <c r="DB117" s="1"/>
-      <c r="DC117" s="4"/>
-      <c r="DD117" s="4"/>
-      <c r="DE117" s="4"/>
-      <c r="DF117" s="4"/>
-      <c r="DG117" s="4"/>
-      <c r="DH117" s="4"/>
-      <c r="DI117" s="4"/>
-      <c r="DJ117" s="4"/>
-      <c r="DK117" s="4"/>
-      <c r="DL117" s="4"/>
-      <c r="DM117" s="4"/>
-      <c r="DN117" s="4"/>
+      <c r="DC117" s="3"/>
+      <c r="DD117" s="3"/>
+      <c r="DE117" s="3"/>
+      <c r="DF117" s="3"/>
+      <c r="DG117" s="3"/>
+      <c r="DH117" s="3"/>
+      <c r="DI117" s="3"/>
+      <c r="DJ117" s="3"/>
+      <c r="DK117" s="3"/>
+      <c r="DL117" s="3"/>
+      <c r="DM117" s="3"/>
+      <c r="DN117" s="3"/>
       <c r="DO117" s="1"/>
     </row>
     <row r="118" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV118" s="7"/>
-      <c r="CW118" s="7"/>
-      <c r="CX118" s="7"/>
-      <c r="CY118" s="7"/>
-      <c r="CZ118" s="7"/>
-      <c r="DA118" s="7"/>
+      <c r="CV118" s="3"/>
+      <c r="CW118" s="3"/>
+      <c r="CX118" s="3"/>
+      <c r="CY118" s="3"/>
+      <c r="CZ118" s="3"/>
+      <c r="DA118" s="3"/>
       <c r="DB118" s="1"/>
-      <c r="DC118" s="4"/>
-      <c r="DD118" s="4"/>
-      <c r="DE118" s="4"/>
-      <c r="DF118" s="4"/>
-      <c r="DG118" s="4"/>
-      <c r="DH118" s="4"/>
-      <c r="DI118" s="4"/>
-      <c r="DJ118" s="4"/>
-      <c r="DK118" s="4"/>
-      <c r="DL118" s="4"/>
-      <c r="DM118" s="4"/>
-      <c r="DN118" s="4"/>
+      <c r="DC118" s="3"/>
+      <c r="DD118" s="3"/>
+      <c r="DE118" s="3"/>
+      <c r="DF118" s="3"/>
+      <c r="DG118" s="3"/>
+      <c r="DH118" s="3"/>
+      <c r="DI118" s="3"/>
+      <c r="DJ118" s="3"/>
+      <c r="DK118" s="3"/>
+      <c r="DL118" s="3"/>
+      <c r="DM118" s="3"/>
+      <c r="DN118" s="3"/>
       <c r="DO118" s="1"/>
     </row>
     <row r="119" spans="100:119" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="CV119" s="7"/>
-      <c r="CW119" s="7"/>
-      <c r="CX119" s="7"/>
-      <c r="CY119" s="7"/>
-      <c r="CZ119" s="7"/>
-      <c r="DA119" s="7"/>
+      <c r="CV119" s="3"/>
+      <c r="CW119" s="3"/>
+      <c r="CX119" s="3"/>
+      <c r="CY119" s="3"/>
+      <c r="CZ119" s="3"/>
+      <c r="DA119" s="3"/>
       <c r="DB119" s="1"/>
       <c r="DC119" s="1"/>
       <c r="DD119" s="1"/>

</xml_diff>